<commit_message>
- added new counterfactual memes
</commit_message>
<xml_diff>
--- a/annotations.xlsx
+++ b/annotations.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>ID</t>
   </si>
@@ -40,13 +40,22 @@
     <t>DaveChappelle-1.jpg</t>
   </si>
   <si>
+    <t>ChrisEvans-Counterf1.jpeg</t>
+  </si>
+  <si>
     <t>Supporting</t>
   </si>
   <si>
     <t>Need</t>
   </si>
   <si>
+    <t>None</t>
+  </si>
+  <si>
     <t>Not hateful</t>
+  </si>
+  <si>
+    <t>Hateful</t>
   </si>
 </sst>
 </file>
@@ -404,7 +413,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -432,10 +441,10 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
@@ -446,10 +455,10 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
@@ -460,12 +469,26 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="b">
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- modified annotation-tool: new scale
</commit_message>
<xml_diff>
--- a/annotations.xlsx
+++ b/annotations.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>ID</t>
   </si>
@@ -22,7 +22,7 @@
     <t>Image-text relation</t>
   </si>
   <si>
-    <t>Hate</t>
+    <t>Hatefulness scale</t>
   </si>
   <si>
     <t>Discard</t>
@@ -37,25 +37,13 @@
     <t>RoseanneBarr-1.jpg</t>
   </si>
   <si>
-    <t>DaveChappelle-1.jpg</t>
-  </si>
-  <si>
-    <t>ChrisEvans-Counterf1.jpeg</t>
-  </si>
-  <si>
-    <t>Supporting</t>
-  </si>
-  <si>
-    <t>Need</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>Not hateful</t>
-  </si>
-  <si>
-    <t>Hateful</t>
+    <t>neutral</t>
+  </si>
+  <si>
+    <t>0 - Non hateful</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
 </sst>
 </file>
@@ -413,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -441,10 +429,10 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
@@ -455,40 +443,12 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- modified annotation-tool: added timer function, added counterparts
</commit_message>
<xml_diff>
--- a/annotations.xlsx
+++ b/annotations.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmehrabanian/PycharmProjects/hatespeech_annotation/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BFB6C20-D24D-CB47-A562-198FAD9064B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="3420" yWindow="500" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>ID</t>
   </si>
@@ -22,35 +28,29 @@
     <t>Image-text relation</t>
   </si>
   <si>
+    <t>checkbox</t>
+  </si>
+  <si>
+    <t>Decision part</t>
+  </si>
+  <si>
     <t>Hatefulness scale</t>
   </si>
   <si>
+    <t>Confidence score</t>
+  </si>
+  <si>
     <t>Discard</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>JosephGoebbels-1.jpg</t>
-  </si>
-  <si>
-    <t>RoseanneBarr-1.jpg</t>
-  </si>
-  <si>
-    <t>neutral</t>
-  </si>
-  <si>
-    <t>0 - Non hateful</t>
-  </si>
-  <si>
-    <t>2</t>
+    <t>Elapsed Time (s)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,13 +113,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -157,7 +165,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -191,6 +199,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -225,9 +234,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -400,14 +410,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="A2:H4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -423,33 +435,14 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="b">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- modified annotation-tool: divided datasets in four parts (dataset1, dataset2, dataset3, dataset4), added upload button to Dropbox via API
</commit_message>
<xml_diff>
--- a/annotations.xlsx
+++ b/annotations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmehrabanian/PycharmProjects/hatespeech_annotation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BFB6C20-D24D-CB47-A562-198FAD9064B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28694774-5953-7341-80F2-CE057E14CF6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3420" yWindow="500" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>

<commit_message>
Modified annotation tool: - added two sections: Introduction and Meme annotation - one meme at one time to speed the annotation process up - added next button - changed image text relation and also added Modality contributes towards hate
</commit_message>
<xml_diff>
--- a/annotations.xlsx
+++ b/annotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmehrabanian/PycharmProjects/hatespeech_annotation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F95C39EC-8C87-2545-BE64-F7A961F5D89D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{716D3B06-F109-9C41-8805-4FDA5E1F6147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3420" yWindow="500" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
     <t>Image-text relation</t>
   </si>
   <si>
-    <t>checkbox</t>
+    <t>Modality towards hate</t>
   </si>
   <si>
     <t>Decision part</t>
@@ -414,7 +414,7 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="A2:H4"/>
+      <selection activeCell="H3" sqref="A2:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
some changes on the instructions
</commit_message>
<xml_diff>
--- a/annotations.xlsx
+++ b/annotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmehrabanian/PycharmProjects/hatespeech_annotation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D421CC-9AA3-C94C-AF2E-FA8C076D59DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C65627A-9A64-B444-B31D-9E86BA678B61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3420" yWindow="500" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -414,7 +414,7 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="A2:H3"/>
+      <selection activeCell="H2" sqref="A2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
- removed preview and replaced it with meme example and annotation video - button, which shows up after the user downloaded the guidelines - added some details about annotating in the pdf file - layout and technical modification
</commit_message>
<xml_diff>
--- a/annotations.xlsx
+++ b/annotations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmehrabanian/PycharmProjects/hatespeech_annotation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C65627A-9A64-B444-B31D-9E86BA678B61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F73FCCA7-F915-BB4B-B268-1186BD7D68F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3420" yWindow="500" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -414,7 +414,7 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="A2:H2"/>
+      <selection activeCell="H3" sqref="A2:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
- added dropbox token button to generate token anytime and updated instructions
</commit_message>
<xml_diff>
--- a/annotations.xlsx
+++ b/annotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmehrabanian/PycharmProjects/hatespeech_annotation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F73FCCA7-F915-BB4B-B268-1186BD7D68F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD9817D8-33C1-7E4A-951D-D0CDD08AD3CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3420" yWindow="500" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -414,7 +414,7 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="A2:H3"/>
+      <selection activeCell="H2" sqref="A2:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>